<commit_message>
update PMP responsibility and communication section& update SIQ
</commit_message>
<xml_diff>
--- a/Requirement/REQ_SIQ_Response.xlsx
+++ b/Requirement/REQ_SIQ_Response.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="102">
   <si>
     <t>Module Name</t>
   </si>
@@ -305,84 +305,55 @@
     <t>SIQ_user_reg_13</t>
   </si>
   <si>
-    <t>Account has - Balance
+    <t>SIQ_user_account_08</t>
+  </si>
+  <si>
+    <t>SIQ_user_transaction_09</t>
+  </si>
+  <si>
+    <t>Users can register using the online registration form only if he has at least one Banking account(حساب بنكى) which is created by the admin for the first time?</t>
+  </si>
+  <si>
+    <t>SIQ_AdminFeatures_02</t>
+  </si>
+  <si>
+    <t>SIQ_AdminFeatures_03</t>
+  </si>
+  <si>
+    <t>SIQ_AdminFeatures_04</t>
+  </si>
+  <si>
+    <t>user register using username,password,national id?</t>
+  </si>
+  <si>
+    <t>Admin can delete user if all bank accounts are deleted?</t>
+  </si>
+  <si>
+    <t>when user successfully registered will be redirected to the  home page?if no please write a comment</t>
+  </si>
+  <si>
+    <t>all user accounts are connected so the user will have one user name and password to use for access all his accounts</t>
+  </si>
+  <si>
+    <t>Admin can edit user account balance ,user password and transaction ?please mention if he can view only</t>
+  </si>
+  <si>
+    <t>Account attributes are only:
+                     - Balance
                      - Transactions History 
                      - Account Number (Unique)
                      - Account Type</t>
   </si>
   <si>
-    <t>SIQ_user_account_08</t>
-  </si>
-  <si>
-    <t>SIQ_user_transaction_09</t>
-  </si>
-  <si>
-    <t>SIQ_user_deletion_10</t>
-  </si>
-  <si>
-    <t>Admin can delete the user after 1 month with a balance less than zero
-if not, please specify the period of time to delete the account</t>
-  </si>
-  <si>
-    <t>Users can register using the online registration form only if he has at least one Banking account(حساب بنكى) which is created by the admin for the first time?</t>
-  </si>
-  <si>
-    <t>SIQ_user_reg_14</t>
-  </si>
-  <si>
-    <t>SIQ_AdminFeatures_02</t>
-  </si>
-  <si>
-    <t>SIQ_AdminFeatures_03</t>
-  </si>
-  <si>
-    <t>SIQ_AdminFeatures_04</t>
-  </si>
-  <si>
-    <t>SIQ_AdminFeatures_05</t>
-  </si>
-  <si>
-    <t>SIQ_AdminFeatures_06</t>
-  </si>
-  <si>
-    <t>Admin can edit user account balance ?</t>
-  </si>
-  <si>
-    <t>Admin can edit user account transaction?</t>
-  </si>
-  <si>
-    <t>Admin can view only user account balance ?</t>
-  </si>
-  <si>
-    <t>Admin can edit only the user password?</t>
-  </si>
-  <si>
-    <t>user register using username,password,national id?</t>
-  </si>
-  <si>
-    <t>when user successfully registered will be redirected to the  home page?</t>
-  </si>
-  <si>
-    <t>when user successfully registered will be redirected to the  login page?</t>
-  </si>
-  <si>
-    <t>user logged in first ,then choose which account to use</t>
-  </si>
-  <si>
-    <t>SIQ_AdminFeatures_07</t>
-  </si>
-  <si>
-    <t>Admin can delete user if all bank accounts are deleted?</t>
-  </si>
-  <si>
-    <t>Admin can delete user ?</t>
-  </si>
-  <si>
-    <t>Each Transaction has 
+    <t>Each Transaction attributes are only:
                      - Trans ID
                      - Amount
                      - Type
                      - Transaction Balance (total account balance after transaction)</t>
+  </si>
+  <si>
+    <t>Admin can delete the user after 1 month with a balance less than zero
+if not, please specify the period of time to delete the accoun</t>
   </si>
 </sst>
 </file>
@@ -604,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -676,30 +647,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -743,15 +690,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -768,15 +706,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -793,14 +722,53 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1020,10 +988,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1015"/>
+  <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1079,7 +1047,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="27" t="s">
@@ -1091,7 +1059,7 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="66" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="6"/>
@@ -1100,7 +1068,7 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
+      <c r="A3" s="78"/>
       <c r="B3" s="28" t="s">
         <v>14</v>
       </c>
@@ -1110,14 +1078,14 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="34"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="20"/>
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
+      <c r="A4" s="78"/>
       <c r="B4" s="28" t="s">
         <v>17</v>
       </c>
@@ -1134,7 +1102,7 @@
       <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:26" ht="84" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
+      <c r="A5" s="78"/>
       <c r="B5" s="28" t="s">
         <v>19</v>
       </c>
@@ -1151,7 +1119,7 @@
       <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
+      <c r="A6" s="78"/>
       <c r="B6" s="28" t="s">
         <v>81</v>
       </c>
@@ -1168,7 +1136,7 @@
       <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:26" ht="70" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1186,8 +1154,8 @@
       <c r="H7" s="20"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:26" ht="28" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.25">
+      <c r="A8" s="78"/>
       <c r="B8" s="28" t="s">
         <v>24</v>
       </c>
@@ -1205,469 +1173,568 @@
       <c r="H8" s="20"/>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:26" s="47" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
-      <c r="B9" s="39" t="s">
+    <row r="9" spans="1:26" s="39" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A9" s="78"/>
+      <c r="B9" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
-      <c r="U9" s="46"/>
-      <c r="V9" s="46"/>
-      <c r="W9" s="46"/>
-      <c r="X9" s="46"/>
-      <c r="Y9" s="46"/>
-      <c r="Z9" s="46"/>
-    </row>
-    <row r="10" spans="1:26" s="47" customFormat="1" ht="28" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
-      <c r="B10" s="41" t="s">
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="38"/>
+    </row>
+    <row r="10" spans="1:26" s="39" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A10" s="78"/>
+      <c r="B10" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="46"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="46"/>
-      <c r="W10" s="46"/>
-      <c r="X10" s="46"/>
-      <c r="Y10" s="46"/>
-      <c r="Z10" s="46"/>
-    </row>
-    <row r="11" spans="1:26" s="47" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
-      <c r="B11" s="41" t="s">
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38"/>
+      <c r="V10" s="38"/>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+    </row>
+    <row r="11" spans="1:26" s="39" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A11" s="78"/>
+      <c r="B11" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="49"/>
-    </row>
-    <row r="12" spans="1:26" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="61" t="s">
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
+    </row>
+    <row r="12" spans="1:26" s="49" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A12" s="78"/>
+      <c r="B12" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="62" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="66"/>
-    </row>
-    <row r="13" spans="1:26" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="61" t="s">
+      <c r="C12" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="55"/>
+    </row>
+    <row r="13" spans="1:26" s="49" customFormat="1" ht="28" x14ac:dyDescent="0.25">
+      <c r="A13" s="78"/>
+      <c r="B13" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="62" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" s="61"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="66"/>
-    </row>
-    <row r="14" spans="1:26" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
-      <c r="B14" s="61" t="s">
+      <c r="C13" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="50"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
+    </row>
+    <row r="14" spans="1:26" s="49" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="A14" s="79"/>
+      <c r="B14" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="61"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="66"/>
-    </row>
-    <row r="15" spans="1:26" s="57" customFormat="1" ht="42" x14ac:dyDescent="0.25">
-      <c r="A15" s="60"/>
-      <c r="B15" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="62" t="s">
+      <c r="C14" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="55"/>
+    </row>
+    <row r="15" spans="1:26" s="39" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A15" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+    </row>
+    <row r="16" spans="1:26" s="39" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A16" s="70"/>
+      <c r="B16" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
+    </row>
+    <row r="17" spans="1:26" s="39" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="70"/>
+      <c r="B17" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="41"/>
+    </row>
+    <row r="18" spans="1:26" s="39" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A18" s="70"/>
+      <c r="B18" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
+    </row>
+    <row r="19" spans="1:26" s="39" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A19" s="70"/>
+      <c r="B19" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
+    </row>
+    <row r="20" spans="1:26" s="49" customFormat="1" ht="28" x14ac:dyDescent="0.25">
+      <c r="A20" s="71"/>
+      <c r="B20" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="42"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="48"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+    </row>
+    <row r="21" spans="1:26" ht="112" x14ac:dyDescent="0.25">
+      <c r="A21" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:26" s="49" customFormat="1" ht="28" x14ac:dyDescent="0.25">
+      <c r="A22" s="75"/>
+      <c r="B22" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="50"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="55"/>
+    </row>
+    <row r="23" spans="1:26" s="49" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A23" s="75"/>
+      <c r="B23" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="50"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="55"/>
+    </row>
+    <row r="24" spans="1:26" s="49" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="75"/>
+      <c r="B24" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="66"/>
-    </row>
-    <row r="16" spans="1:26" s="47" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="41" t="s">
+      <c r="C24" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="55"/>
+    </row>
+    <row r="25" spans="1:26" ht="14" x14ac:dyDescent="0.25">
+      <c r="A25" s="76"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:26" s="5" customFormat="1" ht="27.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="1:26" s="5" customFormat="1" ht="27.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="65"/>
+      <c r="B27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="1:26" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.25">
+      <c r="A28" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="49"/>
-    </row>
-    <row r="17" spans="1:26" s="47" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="41" t="s">
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+    </row>
+    <row r="29" spans="1:26" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="73"/>
+      <c r="B29" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="49"/>
-    </row>
-    <row r="18" spans="1:26" s="47" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="49"/>
-    </row>
-    <row r="19" spans="1:26" s="47" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="41" t="s">
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="9"/>
+    </row>
+    <row r="30" spans="1:26" s="5" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="73"/>
+      <c r="B30" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="49"/>
-    </row>
-    <row r="20" spans="1:26" s="47" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="41" t="s">
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="9"/>
+      <c r="Z30" s="9"/>
+    </row>
+    <row r="31" spans="1:26" s="5" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="73"/>
+      <c r="B31" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="46"/>
-      <c r="P20" s="46"/>
-      <c r="Q20" s="46"/>
-      <c r="R20" s="46"/>
-      <c r="S20" s="46"/>
-      <c r="T20" s="46"/>
-      <c r="U20" s="46"/>
-      <c r="V20" s="46"/>
-      <c r="W20" s="46"/>
-      <c r="X20" s="46"/>
-      <c r="Y20" s="46"/>
-      <c r="Z20" s="46"/>
-    </row>
-    <row r="21" spans="1:26" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="56"/>
-      <c r="T21" s="56"/>
-      <c r="U21" s="56"/>
-      <c r="V21" s="56"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="56"/>
-      <c r="Y21" s="56"/>
-      <c r="Z21" s="56"/>
-    </row>
-    <row r="22" spans="1:26" ht="112" x14ac:dyDescent="0.25">
-      <c r="A22" s="78" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+    </row>
+    <row r="32" spans="1:26" s="5" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="73"/>
+      <c r="B32" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="1:26" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A23" s="80"/>
-      <c r="B23" s="61" t="s">
-        <v>95</v>
-      </c>
-      <c r="C23" s="62" t="s">
-        <v>100</v>
-      </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="66"/>
-    </row>
-    <row r="24" spans="1:26" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A24" s="80"/>
-      <c r="B24" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="66"/>
-    </row>
-    <row r="25" spans="1:26" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A25" s="80"/>
-      <c r="B25" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="66"/>
-    </row>
-    <row r="26" spans="1:26" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A26" s="80"/>
-      <c r="B26" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="66"/>
-    </row>
-    <row r="27" spans="1:26" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A27" s="80"/>
-      <c r="B27" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="62" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="66"/>
-    </row>
-    <row r="28" spans="1:26" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A28" s="80"/>
-      <c r="B28" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="62" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="61"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="66"/>
-    </row>
-    <row r="29" spans="1:26" ht="14" x14ac:dyDescent="0.25">
-      <c r="A29" s="80"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="11"/>
-    </row>
-    <row r="30" spans="1:26" ht="14" x14ac:dyDescent="0.25">
-      <c r="A30" s="79"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="1:26" s="5" customFormat="1" ht="27.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="1:26" s="5" customFormat="1" ht="27.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="12"/>
-    </row>
-    <row r="33" spans="1:26" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
-        <v>53</v>
-      </c>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="9"/>
+      <c r="Z32" s="9"/>
+    </row>
+    <row r="33" spans="1:26" s="5" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="73"/>
       <c r="B33" s="21" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>16</v>
@@ -1695,13 +1762,13 @@
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
     </row>
-    <row r="34" spans="1:26" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="68"/>
+    <row r="34" spans="1:26" s="5" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="73"/>
       <c r="B34" s="21" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>16</v>
@@ -1729,347 +1796,151 @@
       <c r="Y34" s="9"/>
       <c r="Z34" s="9"/>
     </row>
-    <row r="35" spans="1:26" s="5" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="68"/>
-      <c r="B35" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9"/>
-      <c r="Y35" s="9"/>
-      <c r="Z35" s="9"/>
-    </row>
-    <row r="36" spans="1:26" s="5" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="68"/>
-      <c r="B36" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8"/>
-      <c r="W36" s="9"/>
-      <c r="X36" s="9"/>
-      <c r="Y36" s="9"/>
-      <c r="Z36" s="9"/>
-    </row>
-    <row r="37" spans="1:26" s="5" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="68"/>
-      <c r="B37" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>63</v>
+    <row r="35" spans="1:26" s="63" customFormat="1" ht="101.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="73"/>
+      <c r="B35" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="58"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="61"/>
+      <c r="L35" s="61"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="61"/>
+      <c r="O35" s="61"/>
+      <c r="P35" s="61"/>
+      <c r="Q35" s="61"/>
+      <c r="R35" s="61"/>
+      <c r="S35" s="61"/>
+      <c r="T35" s="61"/>
+      <c r="U35" s="61"/>
+      <c r="V35" s="61"/>
+      <c r="W35" s="62"/>
+      <c r="X35" s="62"/>
+      <c r="Y35" s="62"/>
+      <c r="Z35" s="62"/>
+    </row>
+    <row r="36" spans="1:26" s="63" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="73"/>
+      <c r="B36" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="58"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="61"/>
+      <c r="L36" s="61"/>
+      <c r="M36" s="61"/>
+      <c r="N36" s="61"/>
+      <c r="O36" s="61"/>
+      <c r="P36" s="61"/>
+      <c r="Q36" s="61"/>
+      <c r="R36" s="61"/>
+      <c r="S36" s="61"/>
+      <c r="T36" s="61"/>
+      <c r="U36" s="61"/>
+      <c r="V36" s="61"/>
+      <c r="W36" s="62"/>
+      <c r="X36" s="62"/>
+      <c r="Y36" s="62"/>
+      <c r="Z36" s="62"/>
+    </row>
+    <row r="37" spans="1:26" s="5" customFormat="1" ht="31.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>70</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="8"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="9"/>
+      <c r="V37" s="9"/>
       <c r="W37" s="9"/>
       <c r="X37" s="9"/>
       <c r="Y37" s="9"/>
       <c r="Z37" s="9"/>
     </row>
-    <row r="38" spans="1:26" s="5" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="68"/>
-      <c r="B38" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>65</v>
+    <row r="38" spans="1:26" s="5" customFormat="1" ht="25.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="65"/>
+      <c r="B38" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>72</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="9"/>
+      <c r="V38" s="9"/>
       <c r="W38" s="9"/>
       <c r="X38" s="9"/>
       <c r="Y38" s="9"/>
       <c r="Z38" s="9"/>
     </row>
-    <row r="39" spans="1:26" s="5" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="68"/>
-      <c r="B39" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="9"/>
-      <c r="X39" s="9"/>
-      <c r="Y39" s="9"/>
-      <c r="Z39" s="9"/>
-    </row>
-    <row r="40" spans="1:26" s="77" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="68"/>
-      <c r="B40" s="70" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="71" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="72"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="73"/>
-      <c r="I40" s="74"/>
-      <c r="J40" s="75"/>
-      <c r="K40" s="75"/>
-      <c r="L40" s="75"/>
-      <c r="M40" s="75"/>
-      <c r="N40" s="75"/>
-      <c r="O40" s="75"/>
-      <c r="P40" s="75"/>
-      <c r="Q40" s="75"/>
-      <c r="R40" s="75"/>
-      <c r="S40" s="75"/>
-      <c r="T40" s="75"/>
-      <c r="U40" s="75"/>
-      <c r="V40" s="75"/>
-      <c r="W40" s="76"/>
-      <c r="X40" s="76"/>
-      <c r="Y40" s="76"/>
-      <c r="Z40" s="76"/>
-    </row>
-    <row r="41" spans="1:26" s="77" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="68"/>
-      <c r="B41" s="70" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" s="71" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" s="72"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="73"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
-      <c r="M41" s="75"/>
-      <c r="N41" s="75"/>
-      <c r="O41" s="75"/>
-      <c r="P41" s="75"/>
-      <c r="Q41" s="75"/>
-      <c r="R41" s="75"/>
-      <c r="S41" s="75"/>
-      <c r="T41" s="75"/>
-      <c r="U41" s="75"/>
-      <c r="V41" s="75"/>
-      <c r="W41" s="76"/>
-      <c r="X41" s="76"/>
-      <c r="Y41" s="76"/>
-      <c r="Z41" s="76"/>
-    </row>
-    <row r="42" spans="1:26" s="77" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="69"/>
-      <c r="B42" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" s="71" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="72"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="75"/>
-      <c r="K42" s="75"/>
-      <c r="L42" s="75"/>
-      <c r="M42" s="75"/>
-      <c r="N42" s="75"/>
-      <c r="O42" s="75"/>
-      <c r="P42" s="75"/>
-      <c r="Q42" s="75"/>
-      <c r="R42" s="75"/>
-      <c r="S42" s="75"/>
-      <c r="T42" s="75"/>
-      <c r="U42" s="75"/>
-      <c r="V42" s="75"/>
-      <c r="W42" s="76"/>
-      <c r="X42" s="76"/>
-      <c r="Y42" s="76"/>
-      <c r="Z42" s="76"/>
-    </row>
-    <row r="43" spans="1:26" s="5" customFormat="1" ht="31.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="9"/>
-      <c r="T43" s="9"/>
-      <c r="U43" s="9"/>
-      <c r="V43" s="9"/>
-      <c r="W43" s="9"/>
-      <c r="X43" s="9"/>
-      <c r="Y43" s="9"/>
-      <c r="Z43" s="9"/>
-    </row>
-    <row r="44" spans="1:26" s="5" customFormat="1" ht="25.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-      <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
-      <c r="V44" s="9"/>
-      <c r="W44" s="9"/>
-      <c r="X44" s="9"/>
-      <c r="Y44" s="9"/>
-      <c r="Z44" s="9"/>
-    </row>
-    <row r="45" spans="1:26" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-    </row>
+    <row r="39" spans="1:26" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+    </row>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3034,24 +2905,18 @@
     <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A37:A38"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A33:A42"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A28:A36"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A2:A14"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D44">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D38">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>